<commit_message>
Final lit review results
</commit_message>
<xml_diff>
--- a/cleaned lit review results.xlsx
+++ b/cleaned lit review results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66015F79-5ED7-8045-9423-AA69CC92C2E6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AB0FC6-BD3D-9841-B090-CC439C98D461}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="1380" windowWidth="17320" windowHeight="12900" xr2:uid="{6572F45F-1008-5345-97C2-68802297C706}"/>
+    <workbookView xWindow="11480" yWindow="680" windowWidth="17320" windowHeight="12900" xr2:uid="{6572F45F-1008-5345-97C2-68802297C706}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094E9D58-D3DF-3440-9862-D36736538020}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1258,11 +1258,11 @@
         <v>746</v>
       </c>
       <c r="E7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1280,11 +1280,11 @@
         <v>697</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1324,11 +1324,11 @@
         <v>476</v>
       </c>
       <c r="E10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>